<commit_message>
<committed details.> 1) in progress - update modeling: voting Regressor - EDA - GradientBoosting
2) Done
-
</commit_message>
<xml_diff>
--- a/Griffin_r01/meas_setting_4DVE_1st_LUT.xlsx
+++ b/Griffin_r01/meas_setting_4DVE_1st_LUT.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FABA4F3C-AF6E-4B3B-952C-461F772D040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meas_setting_4DVE_1st_LUT" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meas_setting_4DVE_1st_LUT!$A$1:$AB$153</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -118,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,11 +1074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G49" workbookViewId="0">
-      <selection activeCell="AB70" sqref="AB70"/>
+      <selection activeCell="AB75" sqref="AB75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -14263,7 +14274,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB153"/>
+  <autoFilter ref="A1:AB153" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
<committed details.> 1) in progress - update modeling: voting Regressor - EDA
2) Done
- - GridSearchCV
</commit_message>
<xml_diff>
--- a/Griffin_r01/meas_setting_4DVE_1st_LUT.xlsx
+++ b/Griffin_r01/meas_setting_4DVE_1st_LUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthineersapc-my.sharepoint.com/personal/inseop_hwang_siemens-healthineers_com/Documents/1_External Training/2_Python/PycharmProjects/AOP_ML/Griffin_r01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:40009_{FABA4F3C-AF6E-4B3B-952C-461F772D040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A350DC84-1D81-4E0B-A732-1CFE6463D403}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:40009_{FABA4F3C-AF6E-4B3B-952C-461F772D040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66351850-7E13-417C-BD2C-DA1D66E140E6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meas_setting_4DVE_1st_LUT" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,7 +732,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,6 +741,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1091,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH153"/>
+  <dimension ref="A1:AJ153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA139" sqref="AA139"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -14647,7 +14656,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -14753,7 +14762,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>28</v>
       </c>
@@ -14859,7 +14868,7 @@
         <v>0.70000000000000018</v>
       </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>28</v>
       </c>
@@ -14965,7 +14974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>28</v>
       </c>
@@ -15071,7 +15080,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>28</v>
       </c>
@@ -15177,7 +15186,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>28</v>
       </c>
@@ -15283,7 +15292,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>28</v>
       </c>
@@ -15389,7 +15398,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>28</v>
       </c>
@@ -15495,7 +15504,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>28</v>
       </c>
@@ -15601,7 +15610,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>28</v>
       </c>
@@ -15683,8 +15692,16 @@
       <c r="AA138" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="AC138" s="3">
+        <f>AVERAGE(AC2:AC137)</f>
+        <v>0.72058823529411786</v>
+      </c>
+      <c r="AH138" s="3">
+        <f>AVERAGE(AH2:AH137)</f>
+        <v>0.9897058823529401</v>
+      </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>28</v>
       </c>
@@ -15768,15 +15785,19 @@
         <v>1.6102941176470584</v>
       </c>
       <c r="AC139" s="1">
-        <f>SUM(AC2:AC137)</f>
-        <v>98.000000000000028</v>
+        <f>SUM(AC2:AC138)</f>
+        <v>98.720588235294144</v>
       </c>
       <c r="AH139" s="1">
         <f>SUM(AH2:AH137)</f>
         <v>134.59999999999985</v>
       </c>
+      <c r="AJ139">
+        <f>AH139-AC139</f>
+        <v>35.879411764705708</v>
+      </c>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>28</v>
       </c>
@@ -15856,7 +15877,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>28</v>
       </c>
@@ -15936,7 +15957,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>28</v>
       </c>
@@ -16016,7 +16037,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="143" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>28</v>
       </c>
@@ -16096,7 +16117,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>28</v>
       </c>

</xml_diff>